<commit_message>
Test with a variable production cost
</commit_message>
<xml_diff>
--- a/Instances/01_Lumpy_b2_fe25_en_rk50_ll0_l20_HFalse.xlsx
+++ b/Instances/01_Lumpy_b2_fe25_en_rk50_ll0_l20_HFalse.xlsx
@@ -923,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>1673</v>
       </c>
       <c r="D4" t="n">
         <v>0.0048</v>
@@ -955,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1673</v>
       </c>
       <c r="D5" t="n">
         <v>0.002</v>
@@ -987,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1673</v>
       </c>
       <c r="D6" t="n">
         <v>0.0036</v>
@@ -1019,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1013</v>
       </c>
       <c r="D7" t="n">
         <v>0.026</v>
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="D8" t="n">
         <v>0.0508</v>
@@ -1083,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>301</v>
       </c>
       <c r="D9" t="n">
         <v>0.0248</v>

</xml_diff>